<commit_message>
Dataset modification for word count boxplots added
</commit_message>
<xml_diff>
--- a/Datasets/Classification Report/Classification Report 2nd Analysis.xlsx
+++ b/Datasets/Classification Report/Classification Report 2nd Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Classification Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4F3060-D9D2-4BF8-94D0-B821C4CC1141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238F70B6-6496-4FFB-9861-04E3FA6E8427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{AE472E76-F4BE-4C1B-B212-741E51A51A2C}"/>
+    <workbookView xWindow="-24120" yWindow="3135" windowWidth="24240" windowHeight="17640" xr2:uid="{AE472E76-F4BE-4C1B-B212-741E51A51A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="88">
   <si>
     <t>Textblob NaiveBayes Analyzer</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>0.22</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>avg</t>
   </si>
 </sst>
 </file>
@@ -306,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +322,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,13 +358,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,104 +686,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED607A3-B250-40B1-8E38-70655B986468}">
-  <dimension ref="A1:BC32"/>
+  <dimension ref="A1:BD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AY11" sqref="AY11"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="R1" s="4" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="R1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="Z1" s="4" t="s">
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="Z1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AH1" s="4" t="s">
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AH1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AP1" s="4" t="s">
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AP1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AQ1" s="4"/>
-      <c r="AR1" s="4"/>
-      <c r="AS1" s="4"/>
-      <c r="AT1" s="4"/>
-      <c r="AX1" s="4" t="s">
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AX1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AY1" s="4"/>
-      <c r="AZ1" s="4"/>
-      <c r="BA1" s="4"/>
-      <c r="BB1" s="4"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="4"/>
-      <c r="AS2" s="4"/>
-      <c r="AT2" s="4"/>
-      <c r="AX2" s="4"/>
-      <c r="AY2" s="4"/>
-      <c r="AZ2" s="4"/>
-      <c r="BA2" s="4"/>
-      <c r="BB2" s="4"/>
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
@@ -770,14 +795,14 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J3" t="s">
@@ -789,14 +814,14 @@
       <c r="L3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="4"/>
       <c r="O3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="R3" t="s">
@@ -808,14 +833,14 @@
       <c r="T3" t="s">
         <v>3</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="3"/>
+      <c r="V3" s="4"/>
       <c r="W3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Y3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="Z3" t="s">
@@ -827,14 +852,14 @@
       <c r="AB3" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AC3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="3"/>
+      <c r="AD3" s="4"/>
       <c r="AE3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AG3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="AH3" t="s">
@@ -846,14 +871,14 @@
       <c r="AJ3" t="s">
         <v>3</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AK3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AL3" s="3"/>
+      <c r="AL3" s="4"/>
       <c r="AM3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AO3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="AP3" t="s">
@@ -865,14 +890,14 @@
       <c r="AR3" t="s">
         <v>3</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AS3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AT3" s="3"/>
+      <c r="AT3" s="4"/>
       <c r="AU3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AW3" s="4" t="s">
+      <c r="AW3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="AX3" t="s">
@@ -884,16 +909,16 @@
       <c r="AZ3" t="s">
         <v>3</v>
       </c>
-      <c r="BA3" s="3" t="s">
+      <c r="BA3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="BB3" s="3"/>
+      <c r="BB3" s="4"/>
       <c r="BC3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -903,14 +928,14 @@
       <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="4"/>
       <c r="G4">
         <v>41</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="5"/>
       <c r="J4" t="s">
         <v>6</v>
       </c>
@@ -920,14 +945,14 @@
       <c r="L4" t="s">
         <v>85</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="3"/>
+      <c r="N4" s="4"/>
       <c r="O4">
         <v>41</v>
       </c>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="5"/>
       <c r="R4" t="s">
         <v>6</v>
       </c>
@@ -937,14 +962,14 @@
       <c r="T4" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="V4" s="3"/>
+      <c r="V4" s="4"/>
       <c r="W4">
         <v>41</v>
       </c>
-      <c r="Y4" s="4"/>
+      <c r="Y4" s="5"/>
       <c r="Z4" t="s">
         <v>6</v>
       </c>
@@ -954,14 +979,14 @@
       <c r="AB4" t="s">
         <v>32</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AD4" s="3"/>
+      <c r="AD4" s="4"/>
       <c r="AE4">
         <v>41</v>
       </c>
-      <c r="AG4" s="4"/>
+      <c r="AG4" s="5"/>
       <c r="AH4" t="s">
         <v>6</v>
       </c>
@@ -971,14 +996,14 @@
       <c r="AJ4" t="s">
         <v>32</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AK4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AL4" s="3"/>
+      <c r="AL4" s="4"/>
       <c r="AM4">
         <v>41</v>
       </c>
-      <c r="AO4" s="4"/>
+      <c r="AO4" s="5"/>
       <c r="AP4" t="s">
         <v>6</v>
       </c>
@@ -988,14 +1013,14 @@
       <c r="AR4" t="s">
         <v>39</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AS4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AT4" s="3"/>
+      <c r="AT4" s="4"/>
       <c r="AU4">
         <v>41</v>
       </c>
-      <c r="AW4" s="4"/>
+      <c r="AW4" s="5"/>
       <c r="AX4" t="s">
         <v>6</v>
       </c>
@@ -1005,16 +1030,16 @@
       <c r="AZ4" t="s">
         <v>65</v>
       </c>
-      <c r="BA4" s="3" t="s">
+      <c r="BA4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BB4" s="3"/>
+      <c r="BB4" s="4"/>
       <c r="BC4">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1024,14 +1049,14 @@
       <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="4"/>
       <c r="G5">
         <v>101</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="5"/>
       <c r="J5" t="s">
         <v>9</v>
       </c>
@@ -1041,14 +1066,14 @@
       <c r="L5" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="3"/>
+      <c r="N5" s="4"/>
       <c r="O5">
         <v>101</v>
       </c>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="5"/>
       <c r="R5" t="s">
         <v>9</v>
       </c>
@@ -1058,14 +1083,14 @@
       <c r="T5" t="s">
         <v>27</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="U5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V5" s="3"/>
+      <c r="V5" s="4"/>
       <c r="W5">
         <v>101</v>
       </c>
-      <c r="Y5" s="4"/>
+      <c r="Y5" s="5"/>
       <c r="Z5" t="s">
         <v>9</v>
       </c>
@@ -1075,14 +1100,14 @@
       <c r="AB5" t="s">
         <v>38</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AC5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AD5" s="3"/>
+      <c r="AD5" s="4"/>
       <c r="AE5">
         <v>101</v>
       </c>
-      <c r="AG5" s="4"/>
+      <c r="AG5" s="5"/>
       <c r="AH5" t="s">
         <v>9</v>
       </c>
@@ -1092,14 +1117,14 @@
       <c r="AJ5" t="s">
         <v>66</v>
       </c>
-      <c r="AK5" s="3" t="s">
+      <c r="AK5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AL5" s="3"/>
+      <c r="AL5" s="4"/>
       <c r="AM5">
         <v>101</v>
       </c>
-      <c r="AO5" s="4"/>
+      <c r="AO5" s="5"/>
       <c r="AP5" t="s">
         <v>9</v>
       </c>
@@ -1109,14 +1134,14 @@
       <c r="AR5" t="s">
         <v>47</v>
       </c>
-      <c r="AS5" s="3" t="s">
+      <c r="AS5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AT5" s="3"/>
+      <c r="AT5" s="4"/>
       <c r="AU5">
         <v>101</v>
       </c>
-      <c r="AW5" s="4"/>
+      <c r="AW5" s="5"/>
       <c r="AX5" t="s">
         <v>9</v>
       </c>
@@ -1126,20 +1151,20 @@
       <c r="AZ5" t="s">
         <v>56</v>
       </c>
-      <c r="BA5" s="3" t="s">
+      <c r="BA5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="BB5" s="3"/>
+      <c r="BB5" s="4"/>
       <c r="BC5">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="2"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="5"/>
       <c r="J6" t="s">
         <v>81</v>
       </c>
@@ -1149,14 +1174,14 @@
       <c r="L6" t="s">
         <v>82</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="3"/>
+      <c r="N6" s="4"/>
       <c r="O6" s="2">
         <v>0</v>
       </c>
-      <c r="Q6" s="4"/>
+      <c r="Q6" s="5"/>
       <c r="R6" t="s">
         <v>81</v>
       </c>
@@ -1166,14 +1191,14 @@
       <c r="T6" t="s">
         <v>82</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="V6" s="3"/>
+      <c r="V6" s="4"/>
       <c r="W6" s="2">
         <v>0</v>
       </c>
-      <c r="Y6" s="4"/>
+      <c r="Y6" s="5"/>
       <c r="Z6" t="s">
         <v>81</v>
       </c>
@@ -1183,14 +1208,14 @@
       <c r="AB6" t="s">
         <v>82</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AC6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AD6" s="3"/>
+      <c r="AD6" s="4"/>
       <c r="AE6" s="2">
         <v>0</v>
       </c>
-      <c r="AG6" s="4"/>
+      <c r="AG6" s="5"/>
       <c r="AH6" t="s">
         <v>81</v>
       </c>
@@ -1200,14 +1225,14 @@
       <c r="AJ6" t="s">
         <v>82</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AK6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AL6" s="3"/>
+      <c r="AL6" s="4"/>
       <c r="AM6" s="2">
         <v>0</v>
       </c>
-      <c r="AO6" s="4"/>
+      <c r="AO6" s="5"/>
       <c r="AP6" t="s">
         <v>81</v>
       </c>
@@ -1217,14 +1242,14 @@
       <c r="AR6" t="s">
         <v>82</v>
       </c>
-      <c r="AS6" s="3" t="s">
+      <c r="AS6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AT6" s="3"/>
+      <c r="AT6" s="4"/>
       <c r="AU6" s="2">
         <v>0</v>
       </c>
-      <c r="AW6" s="4"/>
+      <c r="AW6" s="5"/>
       <c r="AX6" t="s">
         <v>81</v>
       </c>
@@ -1234,118 +1259,139 @@
       <c r="AZ6" t="s">
         <v>82</v>
       </c>
-      <c r="BA6" s="3" t="s">
+      <c r="BA6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BB6" s="3"/>
+      <c r="BB6" s="4"/>
       <c r="BC6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="Q7" s="4"/>
+      <c r="Q7" s="5"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
-      <c r="Y7" s="4"/>
+      <c r="Y7" s="5"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
-      <c r="AG7" s="4"/>
+      <c r="AG7" s="5"/>
       <c r="AK7" s="1"/>
       <c r="AL7" s="1"/>
-      <c r="AO7" s="4"/>
+      <c r="AO7" s="5"/>
       <c r="AS7" s="1"/>
       <c r="AT7" s="1"/>
-      <c r="AW7" s="4"/>
+      <c r="AW7" s="5"/>
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="4"/>
       <c r="G8">
         <v>142</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="H8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="5"/>
       <c r="J8" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="3"/>
+      <c r="N8" s="4"/>
       <c r="O8">
         <v>142</v>
       </c>
-      <c r="Q8" s="4"/>
+      <c r="P8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q8" s="5"/>
       <c r="R8" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="U8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="V8" s="3"/>
+      <c r="V8" s="4"/>
       <c r="W8">
         <v>142</v>
       </c>
-      <c r="Y8" s="4"/>
+      <c r="X8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y8" s="5"/>
       <c r="Z8" t="s">
         <v>13</v>
       </c>
-      <c r="AC8" s="3" t="s">
+      <c r="AC8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AD8" s="3"/>
+      <c r="AD8" s="4"/>
       <c r="AE8">
         <v>142</v>
       </c>
-      <c r="AG8" s="4"/>
+      <c r="AF8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG8" s="5"/>
       <c r="AH8" t="s">
         <v>13</v>
       </c>
-      <c r="AK8" s="3" t="s">
+      <c r="AK8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AL8" s="3"/>
+      <c r="AL8" s="4"/>
       <c r="AM8">
         <v>142</v>
       </c>
-      <c r="AO8" s="4"/>
+      <c r="AN8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO8" s="5"/>
       <c r="AP8" t="s">
         <v>13</v>
       </c>
-      <c r="AS8" s="3" t="s">
+      <c r="AS8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AT8" s="3"/>
+      <c r="AT8" s="4"/>
       <c r="AU8">
         <v>142</v>
       </c>
-      <c r="AW8" s="4"/>
+      <c r="AV8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW8" s="5"/>
       <c r="AX8" t="s">
         <v>13</v>
       </c>
-      <c r="BA8" s="3" t="s">
+      <c r="BA8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="BB8" s="3"/>
+      <c r="BB8" s="4"/>
       <c r="BC8">
         <v>142</v>
       </c>
+      <c r="BD8" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -1355,14 +1401,17 @@
       <c r="D9" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="4"/>
       <c r="G9">
         <v>142</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="H9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="5"/>
       <c r="J9" t="s">
         <v>15</v>
       </c>
@@ -1372,14 +1421,17 @@
       <c r="L9" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N9" s="3"/>
+      <c r="N9" s="4"/>
       <c r="O9">
         <v>142</v>
       </c>
-      <c r="Q9" s="4"/>
+      <c r="P9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q9" s="5"/>
       <c r="R9" t="s">
         <v>15</v>
       </c>
@@ -1389,14 +1441,17 @@
       <c r="T9" t="s">
         <v>33</v>
       </c>
-      <c r="U9" s="3" t="s">
+      <c r="U9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="V9" s="3"/>
+      <c r="V9" s="4"/>
       <c r="W9">
         <v>142</v>
       </c>
-      <c r="Y9" s="4"/>
+      <c r="X9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y9" s="5"/>
       <c r="Z9" t="s">
         <v>15</v>
       </c>
@@ -1406,14 +1461,17 @@
       <c r="AB9" t="s">
         <v>32</v>
       </c>
-      <c r="AC9" s="3" t="s">
+      <c r="AC9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AD9" s="3"/>
+      <c r="AD9" s="4"/>
       <c r="AE9">
         <v>142</v>
       </c>
-      <c r="AG9" s="4"/>
+      <c r="AF9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG9" s="5"/>
       <c r="AH9" t="s">
         <v>15</v>
       </c>
@@ -1423,14 +1481,17 @@
       <c r="AJ9" t="s">
         <v>76</v>
       </c>
-      <c r="AK9" s="3" t="s">
+      <c r="AK9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AL9" s="3"/>
+      <c r="AL9" s="4"/>
       <c r="AM9">
         <v>142</v>
       </c>
-      <c r="AO9" s="4"/>
+      <c r="AN9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO9" s="5"/>
       <c r="AP9" t="s">
         <v>15</v>
       </c>
@@ -1440,14 +1501,17 @@
       <c r="AR9" t="s">
         <v>73</v>
       </c>
-      <c r="AS9" s="3" t="s">
+      <c r="AS9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AT9" s="3"/>
+      <c r="AT9" s="4"/>
       <c r="AU9">
         <v>142</v>
       </c>
-      <c r="AW9" s="4"/>
+      <c r="AV9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AW9" s="5"/>
       <c r="AX9" t="s">
         <v>15</v>
       </c>
@@ -1457,16 +1521,19 @@
       <c r="AZ9" t="s">
         <v>61</v>
       </c>
-      <c r="BA9" s="3" t="s">
+      <c r="BA9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BB9" s="3"/>
+      <c r="BB9" s="4"/>
       <c r="BC9">
         <v>142</v>
       </c>
+      <c r="BD9" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -1476,14 +1543,17 @@
       <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="4"/>
       <c r="G10">
         <v>142</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="H10">
+        <v>0.62</v>
+      </c>
+      <c r="I10" s="5"/>
       <c r="J10" t="s">
         <v>18</v>
       </c>
@@ -1493,14 +1563,17 @@
       <c r="L10" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="3"/>
+      <c r="N10" s="6"/>
       <c r="O10">
         <v>142</v>
       </c>
-      <c r="Q10" s="4"/>
+      <c r="P10">
+        <v>0.62</v>
+      </c>
+      <c r="Q10" s="5"/>
       <c r="R10" t="s">
         <v>18</v>
       </c>
@@ -1510,14 +1583,17 @@
       <c r="T10" t="s">
         <v>31</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="U10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V10" s="3"/>
+      <c r="V10" s="6"/>
       <c r="W10">
         <v>142</v>
       </c>
-      <c r="Y10" s="4"/>
+      <c r="X10">
+        <v>0.62</v>
+      </c>
+      <c r="Y10" s="5"/>
       <c r="Z10" t="s">
         <v>18</v>
       </c>
@@ -1527,14 +1603,17 @@
       <c r="AB10" t="s">
         <v>62</v>
       </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AC10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AD10" s="3"/>
+      <c r="AD10" s="6"/>
       <c r="AE10">
         <v>142</v>
       </c>
-      <c r="AG10" s="4"/>
+      <c r="AF10">
+        <v>0.62</v>
+      </c>
+      <c r="AG10" s="5"/>
       <c r="AH10" t="s">
         <v>18</v>
       </c>
@@ -1544,14 +1623,17 @@
       <c r="AJ10" t="s">
         <v>73</v>
       </c>
-      <c r="AK10" s="3" t="s">
+      <c r="AK10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AL10" s="3"/>
+      <c r="AL10" s="4"/>
       <c r="AM10">
         <v>142</v>
       </c>
-      <c r="AO10" s="4"/>
+      <c r="AN10">
+        <v>0.62</v>
+      </c>
+      <c r="AO10" s="5"/>
       <c r="AP10" t="s">
         <v>18</v>
       </c>
@@ -1561,14 +1643,17 @@
       <c r="AR10" t="s">
         <v>67</v>
       </c>
-      <c r="AS10" s="3" t="s">
+      <c r="AS10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AT10" s="3"/>
+      <c r="AT10" s="6"/>
       <c r="AU10">
         <v>142</v>
       </c>
-      <c r="AW10" s="4"/>
+      <c r="AV10">
+        <v>0.62</v>
+      </c>
+      <c r="AW10" s="5"/>
       <c r="AX10" t="s">
         <v>18</v>
       </c>
@@ -1578,92 +1663,95 @@
       <c r="AZ10" t="s">
         <v>10</v>
       </c>
-      <c r="BA10" s="3" t="s">
+      <c r="BA10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="BB10" s="3"/>
+      <c r="BB10" s="6"/>
       <c r="BC10">
         <v>142</v>
       </c>
+      <c r="BD10">
+        <v>0.62</v>
+      </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="R12" s="4" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="R12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="AH12" s="4" t="s">
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="AH12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AI12" s="4"/>
-      <c r="AJ12" s="4"/>
-      <c r="AK12" s="4"/>
-      <c r="AL12" s="4"/>
-      <c r="AP12" s="4" t="s">
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AP12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AQ12" s="4"/>
-      <c r="AR12" s="4"/>
-      <c r="AS12" s="4"/>
-      <c r="AT12" s="4"/>
-      <c r="AX12" s="4" t="s">
+      <c r="AQ12" s="5"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="5"/>
+      <c r="AX12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AY12" s="4"/>
-      <c r="AZ12" s="4"/>
-      <c r="BA12" s="4"/>
-      <c r="BB12" s="4"/>
+      <c r="AY12" s="5"/>
+      <c r="AZ12" s="5"/>
+      <c r="BA12" s="5"/>
+      <c r="BB12" s="5"/>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="AH13" s="4"/>
-      <c r="AI13" s="4"/>
-      <c r="AJ13" s="4"/>
-      <c r="AK13" s="4"/>
-      <c r="AL13" s="4"/>
-      <c r="AP13" s="4"/>
-      <c r="AQ13" s="4"/>
-      <c r="AR13" s="4"/>
-      <c r="AS13" s="4"/>
-      <c r="AT13" s="4"/>
-      <c r="AX13" s="4"/>
-      <c r="AY13" s="4"/>
-      <c r="AZ13" s="4"/>
-      <c r="BA13" s="4"/>
-      <c r="BB13" s="4"/>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="5"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="5"/>
+      <c r="AT13" s="5"/>
+      <c r="AX13" s="5"/>
+      <c r="AY13" s="5"/>
+      <c r="AZ13" s="5"/>
+      <c r="BA13" s="5"/>
+      <c r="BB13" s="5"/>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
@@ -1675,14 +1763,14 @@
       <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J14" t="s">
@@ -1694,14 +1782,14 @@
       <c r="L14" t="s">
         <v>3</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N14" s="3"/>
+      <c r="N14" s="4"/>
       <c r="O14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q14" s="4" t="s">
+      <c r="Q14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="R14" t="s">
@@ -1713,14 +1801,14 @@
       <c r="T14" t="s">
         <v>3</v>
       </c>
-      <c r="U14" s="3" t="s">
+      <c r="U14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V14" s="3"/>
+      <c r="V14" s="4"/>
       <c r="W14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Y14" s="4" t="s">
+      <c r="Y14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="Z14" t="s">
@@ -1732,14 +1820,14 @@
       <c r="AB14" t="s">
         <v>3</v>
       </c>
-      <c r="AC14" s="3" t="s">
+      <c r="AC14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD14" s="3"/>
+      <c r="AD14" s="4"/>
       <c r="AE14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AG14" s="4" t="s">
+      <c r="AG14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="AH14" t="s">
@@ -1751,14 +1839,14 @@
       <c r="AJ14" t="s">
         <v>3</v>
       </c>
-      <c r="AK14" s="3" t="s">
+      <c r="AK14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AL14" s="3"/>
+      <c r="AL14" s="4"/>
       <c r="AM14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AO14" s="4" t="s">
+      <c r="AO14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="AP14" t="s">
@@ -1770,14 +1858,14 @@
       <c r="AR14" t="s">
         <v>3</v>
       </c>
-      <c r="AS14" s="3" t="s">
+      <c r="AS14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AT14" s="3"/>
+      <c r="AT14" s="4"/>
       <c r="AU14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AW14" s="4" t="s">
+      <c r="AW14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="AX14" t="s">
@@ -1789,16 +1877,16 @@
       <c r="AZ14" t="s">
         <v>3</v>
       </c>
-      <c r="BA14" s="3" t="s">
+      <c r="BA14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="BB14" s="3"/>
+      <c r="BB14" s="4"/>
       <c r="BC14" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -1808,14 +1896,14 @@
       <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="4"/>
       <c r="G15">
         <v>44</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="5"/>
       <c r="J15" t="s">
         <v>6</v>
       </c>
@@ -1825,14 +1913,14 @@
       <c r="L15" t="s">
         <v>39</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N15" s="3"/>
+      <c r="N15" s="4"/>
       <c r="O15">
         <v>44</v>
       </c>
-      <c r="Q15" s="4"/>
+      <c r="Q15" s="5"/>
       <c r="R15" t="s">
         <v>6</v>
       </c>
@@ -1842,14 +1930,14 @@
       <c r="T15" t="s">
         <v>68</v>
       </c>
-      <c r="U15" s="3" t="s">
+      <c r="U15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="V15" s="3"/>
+      <c r="V15" s="4"/>
       <c r="W15">
         <v>44</v>
       </c>
-      <c r="Y15" s="4"/>
+      <c r="Y15" s="5"/>
       <c r="Z15" t="s">
         <v>6</v>
       </c>
@@ -1859,14 +1947,14 @@
       <c r="AB15" t="s">
         <v>70</v>
       </c>
-      <c r="AC15" s="3" t="s">
+      <c r="AC15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AD15" s="3"/>
+      <c r="AD15" s="4"/>
       <c r="AE15">
         <v>44</v>
       </c>
-      <c r="AG15" s="4"/>
+      <c r="AG15" s="5"/>
       <c r="AH15" t="s">
         <v>6</v>
       </c>
@@ -1876,14 +1964,14 @@
       <c r="AJ15" t="s">
         <v>78</v>
       </c>
-      <c r="AK15" s="3" t="s">
+      <c r="AK15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AL15" s="3"/>
+      <c r="AL15" s="4"/>
       <c r="AM15">
         <v>44</v>
       </c>
-      <c r="AO15" s="4"/>
+      <c r="AO15" s="5"/>
       <c r="AP15" t="s">
         <v>6</v>
       </c>
@@ -1893,14 +1981,14 @@
       <c r="AR15" t="s">
         <v>63</v>
       </c>
-      <c r="AS15" s="3" t="s">
+      <c r="AS15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AT15" s="3"/>
+      <c r="AT15" s="4"/>
       <c r="AU15">
         <v>44</v>
       </c>
-      <c r="AW15" s="4"/>
+      <c r="AW15" s="5"/>
       <c r="AX15" t="s">
         <v>6</v>
       </c>
@@ -1910,16 +1998,16 @@
       <c r="AZ15" t="s">
         <v>70</v>
       </c>
-      <c r="BA15" s="3" t="s">
+      <c r="BA15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="BB15" s="3"/>
+      <c r="BB15" s="4"/>
       <c r="BC15">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -1929,14 +2017,14 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="4"/>
       <c r="G16">
         <v>23</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="5"/>
       <c r="J16" t="s">
         <v>9</v>
       </c>
@@ -1946,14 +2034,14 @@
       <c r="L16" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="N16" s="4"/>
       <c r="O16">
         <v>23</v>
       </c>
-      <c r="Q16" s="4"/>
+      <c r="Q16" s="5"/>
       <c r="R16" t="s">
         <v>9</v>
       </c>
@@ -1963,14 +2051,14 @@
       <c r="T16" t="s">
         <v>14</v>
       </c>
-      <c r="U16" s="3" t="s">
+      <c r="U16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="V16" s="3"/>
+      <c r="V16" s="4"/>
       <c r="W16">
         <v>23</v>
       </c>
-      <c r="Y16" s="4"/>
+      <c r="Y16" s="5"/>
       <c r="Z16" t="s">
         <v>9</v>
       </c>
@@ -1980,14 +2068,14 @@
       <c r="AB16" t="s">
         <v>14</v>
       </c>
-      <c r="AC16" s="3" t="s">
+      <c r="AC16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AD16" s="3"/>
+      <c r="AD16" s="4"/>
       <c r="AE16">
         <v>23</v>
       </c>
-      <c r="AG16" s="4"/>
+      <c r="AG16" s="5"/>
       <c r="AH16" t="s">
         <v>9</v>
       </c>
@@ -1997,14 +2085,14 @@
       <c r="AJ16" t="s">
         <v>76</v>
       </c>
-      <c r="AK16" s="3" t="s">
+      <c r="AK16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AL16" s="3"/>
+      <c r="AL16" s="4"/>
       <c r="AM16">
         <v>23</v>
       </c>
-      <c r="AO16" s="4"/>
+      <c r="AO16" s="5"/>
       <c r="AP16" t="s">
         <v>9</v>
       </c>
@@ -2014,14 +2102,14 @@
       <c r="AR16" t="s">
         <v>80</v>
       </c>
-      <c r="AS16" s="3" t="s">
+      <c r="AS16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AT16" s="3"/>
+      <c r="AT16" s="4"/>
       <c r="AU16">
         <v>23</v>
       </c>
-      <c r="AW16" s="4"/>
+      <c r="AW16" s="5"/>
       <c r="AX16" t="s">
         <v>9</v>
       </c>
@@ -2031,20 +2119,20 @@
       <c r="AZ16" t="s">
         <v>42</v>
       </c>
-      <c r="BA16" s="3" t="s">
+      <c r="BA16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BB16" s="3"/>
+      <c r="BB16" s="4"/>
       <c r="BC16">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="5"/>
       <c r="J17" t="s">
         <v>81</v>
       </c>
@@ -2054,14 +2142,14 @@
       <c r="L17" t="s">
         <v>82</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="N17" s="3"/>
+      <c r="N17" s="4"/>
       <c r="O17" s="2">
         <v>0</v>
       </c>
-      <c r="Q17" s="4"/>
+      <c r="Q17" s="5"/>
       <c r="R17" t="s">
         <v>81</v>
       </c>
@@ -2071,14 +2159,14 @@
       <c r="T17" t="s">
         <v>82</v>
       </c>
-      <c r="U17" s="3" t="s">
+      <c r="U17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="V17" s="3"/>
+      <c r="V17" s="4"/>
       <c r="W17" s="2">
         <v>0</v>
       </c>
-      <c r="Y17" s="4"/>
+      <c r="Y17" s="5"/>
       <c r="Z17" t="s">
         <v>81</v>
       </c>
@@ -2088,14 +2176,14 @@
       <c r="AB17" t="s">
         <v>82</v>
       </c>
-      <c r="AC17" s="3" t="s">
+      <c r="AC17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AD17" s="3"/>
+      <c r="AD17" s="4"/>
       <c r="AE17" s="2">
         <v>0</v>
       </c>
-      <c r="AG17" s="4"/>
+      <c r="AG17" s="5"/>
       <c r="AH17" t="s">
         <v>81</v>
       </c>
@@ -2105,14 +2193,14 @@
       <c r="AJ17" t="s">
         <v>82</v>
       </c>
-      <c r="AK17" s="3" t="s">
+      <c r="AK17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AL17" s="3"/>
+      <c r="AL17" s="4"/>
       <c r="AM17" s="2">
         <v>0</v>
       </c>
-      <c r="AO17" s="4"/>
+      <c r="AO17" s="5"/>
       <c r="AP17" t="s">
         <v>81</v>
       </c>
@@ -2122,14 +2210,14 @@
       <c r="AR17" t="s">
         <v>82</v>
       </c>
-      <c r="AS17" s="3" t="s">
+      <c r="AS17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AT17" s="3"/>
+      <c r="AT17" s="4"/>
       <c r="AU17" s="2">
         <v>0</v>
       </c>
-      <c r="AW17" s="4"/>
+      <c r="AW17" s="5"/>
       <c r="AX17" t="s">
         <v>81</v>
       </c>
@@ -2139,118 +2227,139 @@
       <c r="AZ17" t="s">
         <v>82</v>
       </c>
-      <c r="BA17" s="3" t="s">
+      <c r="BA17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BB17" s="3"/>
+      <c r="BB17" s="4"/>
       <c r="BC17" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="5"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="Q18" s="4"/>
+      <c r="Q18" s="5"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
-      <c r="Y18" s="4"/>
+      <c r="Y18" s="5"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
-      <c r="AG18" s="4"/>
+      <c r="AG18" s="5"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
-      <c r="AO18" s="4"/>
+      <c r="AO18" s="5"/>
       <c r="AS18" s="1"/>
       <c r="AT18" s="1"/>
-      <c r="AW18" s="4"/>
+      <c r="AW18" s="5"/>
       <c r="BA18" s="1"/>
       <c r="BB18" s="1"/>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="4"/>
       <c r="G19">
         <v>67</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="H19" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="5"/>
       <c r="J19" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N19" s="3"/>
+      <c r="N19" s="4"/>
       <c r="O19">
         <v>67</v>
       </c>
-      <c r="Q19" s="4"/>
+      <c r="P19" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q19" s="5"/>
       <c r="R19" t="s">
         <v>13</v>
       </c>
-      <c r="U19" s="3" t="s">
+      <c r="U19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="V19" s="3"/>
+      <c r="V19" s="4"/>
       <c r="W19">
         <v>67</v>
       </c>
-      <c r="Y19" s="4"/>
+      <c r="X19" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y19" s="5"/>
       <c r="Z19" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="3" t="s">
+      <c r="AC19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AD19" s="3"/>
+      <c r="AD19" s="4"/>
       <c r="AE19">
         <v>67</v>
       </c>
-      <c r="AG19" s="4"/>
+      <c r="AF19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG19" s="5"/>
       <c r="AH19" t="s">
         <v>13</v>
       </c>
-      <c r="AK19" s="3" t="s">
+      <c r="AK19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AL19" s="3"/>
+      <c r="AL19" s="4"/>
       <c r="AM19">
         <v>67</v>
       </c>
-      <c r="AO19" s="4"/>
+      <c r="AN19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO19" s="5"/>
       <c r="AP19" t="s">
         <v>13</v>
       </c>
-      <c r="AS19" s="3" t="s">
+      <c r="AS19" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AT19" s="3"/>
+      <c r="AT19" s="4"/>
       <c r="AU19">
         <v>67</v>
       </c>
-      <c r="AW19" s="4"/>
+      <c r="AV19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW19" s="5"/>
       <c r="AX19" t="s">
         <v>13</v>
       </c>
-      <c r="BA19" s="3" t="s">
+      <c r="BA19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BB19" s="3"/>
+      <c r="BB19" s="4"/>
       <c r="BC19">
         <v>67</v>
       </c>
+      <c r="BD19" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -2260,14 +2369,17 @@
       <c r="D20" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="4"/>
       <c r="G20">
         <v>67</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="H20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="5"/>
       <c r="J20" t="s">
         <v>15</v>
       </c>
@@ -2277,14 +2389,17 @@
       <c r="L20" t="s">
         <v>48</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="M20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N20" s="3"/>
+      <c r="N20" s="4"/>
       <c r="O20">
         <v>67</v>
       </c>
-      <c r="Q20" s="4"/>
+      <c r="P20" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q20" s="5"/>
       <c r="R20" t="s">
         <v>15</v>
       </c>
@@ -2294,14 +2409,17 @@
       <c r="T20" t="s">
         <v>29</v>
       </c>
-      <c r="U20" s="3" t="s">
+      <c r="U20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="V20" s="3"/>
+      <c r="V20" s="4"/>
       <c r="W20">
         <v>67</v>
       </c>
-      <c r="Y20" s="4"/>
+      <c r="X20" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y20" s="5"/>
       <c r="Z20" t="s">
         <v>15</v>
       </c>
@@ -2311,14 +2429,17 @@
       <c r="AB20" t="s">
         <v>11</v>
       </c>
-      <c r="AC20" s="3" t="s">
+      <c r="AC20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AD20" s="3"/>
+      <c r="AD20" s="4"/>
       <c r="AE20">
         <v>67</v>
       </c>
-      <c r="AG20" s="4"/>
+      <c r="AF20" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG20" s="5"/>
       <c r="AH20" t="s">
         <v>15</v>
       </c>
@@ -2328,14 +2449,17 @@
       <c r="AJ20" t="s">
         <v>84</v>
       </c>
-      <c r="AK20" s="3" t="s">
+      <c r="AK20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AL20" s="3"/>
+      <c r="AL20" s="4"/>
       <c r="AM20">
         <v>67</v>
       </c>
-      <c r="AO20" s="4"/>
+      <c r="AN20" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO20" s="5"/>
       <c r="AP20" t="s">
         <v>15</v>
       </c>
@@ -2345,14 +2469,17 @@
       <c r="AR20" t="s">
         <v>66</v>
       </c>
-      <c r="AS20" s="3" t="s">
+      <c r="AS20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AT20" s="3"/>
+      <c r="AT20" s="4"/>
       <c r="AU20">
         <v>67</v>
       </c>
-      <c r="AW20" s="4"/>
+      <c r="AV20" t="s">
+        <v>87</v>
+      </c>
+      <c r="AW20" s="5"/>
       <c r="AX20" t="s">
         <v>15</v>
       </c>
@@ -2362,16 +2489,19 @@
       <c r="AZ20" t="s">
         <v>49</v>
       </c>
-      <c r="BA20" s="3" t="s">
+      <c r="BA20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="BB20" s="3"/>
+      <c r="BB20" s="4"/>
       <c r="BC20">
         <v>67</v>
       </c>
+      <c r="BD20" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -2381,14 +2511,17 @@
       <c r="D21" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="4"/>
       <c r="G21">
         <v>67</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="H21">
+        <v>0.71</v>
+      </c>
+      <c r="I21" s="5"/>
       <c r="J21" t="s">
         <v>18</v>
       </c>
@@ -2398,14 +2531,17 @@
       <c r="L21" t="s">
         <v>36</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="M21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N21" s="3"/>
+      <c r="N21" s="4"/>
       <c r="O21">
         <v>67</v>
       </c>
-      <c r="Q21" s="4"/>
+      <c r="P21">
+        <v>0.71</v>
+      </c>
+      <c r="Q21" s="5"/>
       <c r="R21" t="s">
         <v>18</v>
       </c>
@@ -2415,14 +2551,17 @@
       <c r="T21" t="s">
         <v>62</v>
       </c>
-      <c r="U21" s="3" t="s">
+      <c r="U21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="V21" s="3"/>
+      <c r="V21" s="7"/>
       <c r="W21">
         <v>67</v>
       </c>
-      <c r="Y21" s="4"/>
+      <c r="X21">
+        <v>0.71</v>
+      </c>
+      <c r="Y21" s="5"/>
       <c r="Z21" t="s">
         <v>18</v>
       </c>
@@ -2432,14 +2571,17 @@
       <c r="AB21" t="s">
         <v>35</v>
       </c>
-      <c r="AC21" s="3" t="s">
+      <c r="AC21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AD21" s="3"/>
+      <c r="AD21" s="6"/>
       <c r="AE21">
         <v>67</v>
       </c>
-      <c r="AG21" s="4"/>
+      <c r="AF21">
+        <v>0.71</v>
+      </c>
+      <c r="AG21" s="5"/>
       <c r="AH21" t="s">
         <v>18</v>
       </c>
@@ -2449,14 +2591,17 @@
       <c r="AJ21" t="s">
         <v>49</v>
       </c>
-      <c r="AK21" s="3" t="s">
+      <c r="AK21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AL21" s="3"/>
+      <c r="AL21" s="4"/>
       <c r="AM21">
         <v>67</v>
       </c>
-      <c r="AO21" s="4"/>
+      <c r="AN21">
+        <v>0.71</v>
+      </c>
+      <c r="AO21" s="5"/>
       <c r="AP21" t="s">
         <v>18</v>
       </c>
@@ -2466,14 +2611,17 @@
       <c r="AR21" t="s">
         <v>71</v>
       </c>
-      <c r="AS21" s="3" t="s">
+      <c r="AS21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AT21" s="3"/>
+      <c r="AT21" s="6"/>
       <c r="AU21">
         <v>67</v>
       </c>
-      <c r="AW21" s="4"/>
+      <c r="AV21">
+        <v>0.71</v>
+      </c>
+      <c r="AW21" s="5"/>
       <c r="AX21" t="s">
         <v>18</v>
       </c>
@@ -2483,596 +2631,678 @@
       <c r="AZ21" t="s">
         <v>63</v>
       </c>
-      <c r="BA21" s="3" t="s">
+      <c r="BA21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="BB21" s="3"/>
+      <c r="BB21" s="6"/>
       <c r="BC21">
         <v>67</v>
       </c>
+      <c r="BD21">
+        <v>0.71</v>
+      </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
-      <c r="AB23" s="5"/>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-      <c r="AG23" s="5"/>
-      <c r="AH23" s="5"/>
-      <c r="AI23" s="5"/>
-      <c r="AJ23" s="5"/>
-      <c r="AK23" s="5"/>
-      <c r="AL23" s="5"/>
-      <c r="AM23" s="5"/>
-      <c r="AN23" s="5"/>
-      <c r="AO23" s="5"/>
-      <c r="AP23" s="5"/>
-      <c r="AQ23" s="5"/>
-      <c r="AR23" s="5"/>
-      <c r="AS23" s="5"/>
-      <c r="AT23" s="5"/>
-      <c r="AU23" s="5"/>
-      <c r="AV23" s="5"/>
-      <c r="AW23" s="5"/>
-      <c r="AX23" s="5"/>
-      <c r="AY23" s="5"/>
-      <c r="AZ23" s="5"/>
-      <c r="BA23" s="5"/>
-      <c r="BB23" s="5"/>
-      <c r="BC23" s="5"/>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="V22" s="8"/>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
-      <c r="AB24" s="5"/>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
-      <c r="AG24" s="5"/>
-      <c r="AH24" s="5"/>
-      <c r="AI24" s="5"/>
-      <c r="AJ24" s="5"/>
-      <c r="AK24" s="5"/>
-      <c r="AL24" s="5"/>
-      <c r="AM24" s="5"/>
-      <c r="AN24" s="5"/>
-      <c r="AO24" s="5"/>
-      <c r="AP24" s="5"/>
-      <c r="AQ24" s="5"/>
-      <c r="AR24" s="5"/>
-      <c r="AS24" s="5"/>
-      <c r="AT24" s="5"/>
-      <c r="AU24" s="5"/>
-      <c r="AV24" s="5"/>
-      <c r="AW24" s="5"/>
-      <c r="AX24" s="5"/>
-      <c r="AY24" s="5"/>
-      <c r="AZ24" s="5"/>
-      <c r="BA24" s="5"/>
-      <c r="BB24" s="5"/>
-      <c r="BC24" s="5"/>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+      <c r="AW23" s="3"/>
+      <c r="AX23" s="3"/>
+      <c r="AY23" s="3"/>
+      <c r="AZ23" s="3"/>
+      <c r="BA23" s="3"/>
+      <c r="BB23" s="3"/>
+      <c r="BC23" s="3"/>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
-      <c r="AB25" s="5"/>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-      <c r="AG25" s="5"/>
-      <c r="AH25" s="5"/>
-      <c r="AI25" s="5"/>
-      <c r="AJ25" s="5"/>
-      <c r="AK25" s="5"/>
-      <c r="AL25" s="5"/>
-      <c r="AM25" s="5"/>
-      <c r="AN25" s="5"/>
-      <c r="AO25" s="5"/>
-      <c r="AP25" s="5"/>
-      <c r="AQ25" s="5"/>
-      <c r="AR25" s="5"/>
-      <c r="AS25" s="5"/>
-      <c r="AT25" s="5"/>
-      <c r="AU25" s="5"/>
-      <c r="AV25" s="5"/>
-      <c r="AW25" s="5"/>
-      <c r="AX25" s="5"/>
-      <c r="AY25" s="5"/>
-      <c r="AZ25" s="5"/>
-      <c r="BA25" s="5"/>
-      <c r="BB25" s="5"/>
-      <c r="BC25" s="5"/>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="3"/>
+      <c r="AO24" s="3"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+      <c r="AW24" s="3"/>
+      <c r="AX24" s="3"/>
+      <c r="AY24" s="3"/>
+      <c r="AZ24" s="3"/>
+      <c r="BA24" s="3"/>
+      <c r="BB24" s="3"/>
+      <c r="BC24" s="3"/>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
-      <c r="AG26" s="5"/>
-      <c r="AH26" s="5"/>
-      <c r="AI26" s="5"/>
-      <c r="AJ26" s="5"/>
-      <c r="AK26" s="5"/>
-      <c r="AL26" s="5"/>
-      <c r="AM26" s="5"/>
-      <c r="AN26" s="5"/>
-      <c r="AO26" s="5"/>
-      <c r="AP26" s="5"/>
-      <c r="AQ26" s="5"/>
-      <c r="AR26" s="5"/>
-      <c r="AS26" s="5"/>
-      <c r="AT26" s="5"/>
-      <c r="AU26" s="5"/>
-      <c r="AV26" s="5"/>
-      <c r="AW26" s="5"/>
-      <c r="AX26" s="5"/>
-      <c r="AY26" s="5"/>
-      <c r="AZ26" s="5"/>
-      <c r="BA26" s="5"/>
-      <c r="BB26" s="5"/>
-      <c r="BC26" s="5"/>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="3"/>
+      <c r="AO25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+      <c r="AU25" s="3"/>
+      <c r="AV25" s="3"/>
+      <c r="AW25" s="3"/>
+      <c r="AX25" s="3"/>
+      <c r="AY25" s="3"/>
+      <c r="AZ25" s="3"/>
+      <c r="BA25" s="3"/>
+      <c r="BB25" s="3"/>
+      <c r="BC25" s="3"/>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="5"/>
-      <c r="AB27" s="5"/>
-      <c r="AC27" s="5"/>
-      <c r="AD27" s="5"/>
-      <c r="AE27" s="5"/>
-      <c r="AF27" s="5"/>
-      <c r="AG27" s="5"/>
-      <c r="AH27" s="5"/>
-      <c r="AI27" s="5"/>
-      <c r="AJ27" s="5"/>
-      <c r="AK27" s="5"/>
-      <c r="AL27" s="5"/>
-      <c r="AM27" s="5"/>
-      <c r="AN27" s="5"/>
-      <c r="AO27" s="5"/>
-      <c r="AP27" s="5"/>
-      <c r="AQ27" s="5"/>
-      <c r="AR27" s="5"/>
-      <c r="AS27" s="5"/>
-      <c r="AT27" s="5"/>
-      <c r="AU27" s="5"/>
-      <c r="AV27" s="5"/>
-      <c r="AW27" s="5"/>
-      <c r="AX27" s="5"/>
-      <c r="AY27" s="5"/>
-      <c r="AZ27" s="5"/>
-      <c r="BA27" s="5"/>
-      <c r="BB27" s="5"/>
-      <c r="BC27" s="5"/>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="3"/>
+      <c r="AO26" s="3"/>
+      <c r="AP26" s="3"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+      <c r="AT26" s="3"/>
+      <c r="AU26" s="3"/>
+      <c r="AV26" s="3"/>
+      <c r="AW26" s="3"/>
+      <c r="AX26" s="3"/>
+      <c r="AY26" s="3"/>
+      <c r="AZ26" s="3"/>
+      <c r="BA26" s="3"/>
+      <c r="BB26" s="3"/>
+      <c r="BC26" s="3"/>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
-      <c r="AG28" s="5"/>
-      <c r="AH28" s="5"/>
-      <c r="AI28" s="5"/>
-      <c r="AJ28" s="5"/>
-      <c r="AK28" s="5"/>
-      <c r="AL28" s="5"/>
-      <c r="AM28" s="5"/>
-      <c r="AN28" s="5"/>
-      <c r="AO28" s="5"/>
-      <c r="AP28" s="5"/>
-      <c r="AQ28" s="5"/>
-      <c r="AR28" s="5"/>
-      <c r="AS28" s="5"/>
-      <c r="AT28" s="5"/>
-      <c r="AU28" s="5"/>
-      <c r="AV28" s="5"/>
-      <c r="AW28" s="5"/>
-      <c r="AX28" s="5"/>
-      <c r="AY28" s="5"/>
-      <c r="AZ28" s="5"/>
-      <c r="BA28" s="5"/>
-      <c r="BB28" s="5"/>
-      <c r="BC28" s="5"/>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="3"/>
+      <c r="AO27" s="3"/>
+      <c r="AP27" s="3"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
+      <c r="AT27" s="3"/>
+      <c r="AU27" s="3"/>
+      <c r="AV27" s="3"/>
+      <c r="AW27" s="3"/>
+      <c r="AX27" s="3"/>
+      <c r="AY27" s="3"/>
+      <c r="AZ27" s="3"/>
+      <c r="BA27" s="3"/>
+      <c r="BB27" s="3"/>
+      <c r="BC27" s="3"/>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
-      <c r="AG29" s="5"/>
-      <c r="AH29" s="5"/>
-      <c r="AI29" s="5"/>
-      <c r="AJ29" s="5"/>
-      <c r="AK29" s="5"/>
-      <c r="AL29" s="5"/>
-      <c r="AM29" s="5"/>
-      <c r="AN29" s="5"/>
-      <c r="AO29" s="5"/>
-      <c r="AP29" s="5"/>
-      <c r="AQ29" s="5"/>
-      <c r="AR29" s="5"/>
-      <c r="AS29" s="5"/>
-      <c r="AT29" s="5"/>
-      <c r="AU29" s="5"/>
-      <c r="AV29" s="5"/>
-      <c r="AW29" s="5"/>
-      <c r="AX29" s="5"/>
-      <c r="AY29" s="5"/>
-      <c r="AZ29" s="5"/>
-      <c r="BA29" s="5"/>
-      <c r="BB29" s="5"/>
-      <c r="BC29" s="5"/>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="3"/>
+      <c r="AO28" s="3"/>
+      <c r="AP28" s="3"/>
+      <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
+      <c r="AS28" s="3"/>
+      <c r="AT28" s="3"/>
+      <c r="AU28" s="3"/>
+      <c r="AV28" s="3"/>
+      <c r="AW28" s="3"/>
+      <c r="AX28" s="3"/>
+      <c r="AY28" s="3"/>
+      <c r="AZ28" s="3"/>
+      <c r="BA28" s="3"/>
+      <c r="BB28" s="3"/>
+      <c r="BC28" s="3"/>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="Z30" s="5"/>
-      <c r="AA30" s="5"/>
-      <c r="AB30" s="5"/>
-      <c r="AC30" s="5"/>
-      <c r="AD30" s="5"/>
-      <c r="AE30" s="5"/>
-      <c r="AF30" s="5"/>
-      <c r="AG30" s="5"/>
-      <c r="AH30" s="5"/>
-      <c r="AI30" s="5"/>
-      <c r="AJ30" s="5"/>
-      <c r="AK30" s="5"/>
-      <c r="AL30" s="5"/>
-      <c r="AM30" s="5"/>
-      <c r="AN30" s="5"/>
-      <c r="AO30" s="5"/>
-      <c r="AP30" s="5"/>
-      <c r="AQ30" s="5"/>
-      <c r="AR30" s="5"/>
-      <c r="AS30" s="5"/>
-      <c r="AT30" s="5"/>
-      <c r="AU30" s="5"/>
-      <c r="AV30" s="5"/>
-      <c r="AW30" s="5"/>
-      <c r="AX30" s="5"/>
-      <c r="AY30" s="5"/>
-      <c r="AZ30" s="5"/>
-      <c r="BA30" s="5"/>
-      <c r="BB30" s="5"/>
-      <c r="BC30" s="5"/>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="3"/>
+      <c r="AN29" s="3"/>
+      <c r="AO29" s="3"/>
+      <c r="AP29" s="3"/>
+      <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
+      <c r="AS29" s="3"/>
+      <c r="AT29" s="3"/>
+      <c r="AU29" s="3"/>
+      <c r="AV29" s="3"/>
+      <c r="AW29" s="3"/>
+      <c r="AX29" s="3"/>
+      <c r="AY29" s="3"/>
+      <c r="AZ29" s="3"/>
+      <c r="BA29" s="3"/>
+      <c r="BB29" s="3"/>
+      <c r="BC29" s="3"/>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="5"/>
-      <c r="AG31" s="5"/>
-      <c r="AH31" s="5"/>
-      <c r="AI31" s="5"/>
-      <c r="AJ31" s="5"/>
-      <c r="AK31" s="5"/>
-      <c r="AL31" s="5"/>
-      <c r="AM31" s="5"/>
-      <c r="AN31" s="5"/>
-      <c r="AO31" s="5"/>
-      <c r="AP31" s="5"/>
-      <c r="AQ31" s="5"/>
-      <c r="AR31" s="5"/>
-      <c r="AS31" s="5"/>
-      <c r="AT31" s="5"/>
-      <c r="AU31" s="5"/>
-      <c r="AV31" s="5"/>
-      <c r="AW31" s="5"/>
-      <c r="AX31" s="5"/>
-      <c r="AY31" s="5"/>
-      <c r="AZ31" s="5"/>
-      <c r="BA31" s="5"/>
-      <c r="BB31" s="5"/>
-      <c r="BC31" s="5"/>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
+      <c r="AM30" s="3"/>
+      <c r="AN30" s="3"/>
+      <c r="AO30" s="3"/>
+      <c r="AP30" s="3"/>
+      <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
+      <c r="AS30" s="3"/>
+      <c r="AT30" s="3"/>
+      <c r="AU30" s="3"/>
+      <c r="AV30" s="3"/>
+      <c r="AW30" s="3"/>
+      <c r="AX30" s="3"/>
+      <c r="AY30" s="3"/>
+      <c r="AZ30" s="3"/>
+      <c r="BA30" s="3"/>
+      <c r="BB30" s="3"/>
+      <c r="BC30" s="3"/>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
-      <c r="AB32" s="5"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
-      <c r="AE32" s="5"/>
-      <c r="AF32" s="5"/>
-      <c r="AG32" s="5"/>
-      <c r="AH32" s="5"/>
-      <c r="AI32" s="5"/>
-      <c r="AJ32" s="5"/>
-      <c r="AK32" s="5"/>
-      <c r="AL32" s="5"/>
-      <c r="AM32" s="5"/>
-      <c r="AN32" s="5"/>
-      <c r="AO32" s="5"/>
-      <c r="AP32" s="5"/>
-      <c r="AQ32" s="5"/>
-      <c r="AR32" s="5"/>
-      <c r="AS32" s="5"/>
-      <c r="AT32" s="5"/>
-      <c r="AU32" s="5"/>
-      <c r="AV32" s="5"/>
-      <c r="AW32" s="5"/>
-      <c r="AX32" s="5"/>
-      <c r="AY32" s="5"/>
-      <c r="AZ32" s="5"/>
-      <c r="BA32" s="5"/>
-      <c r="BB32" s="5"/>
-      <c r="BC32" s="5"/>
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="3"/>
+      <c r="AO31" s="3"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+      <c r="AU31" s="3"/>
+      <c r="AV31" s="3"/>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="3"/>
+      <c r="AY31" s="3"/>
+      <c r="AZ31" s="3"/>
+      <c r="BA31" s="3"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="3"/>
+    </row>
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="3"/>
+      <c r="AO32" s="3"/>
+      <c r="AP32" s="3"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="3"/>
+      <c r="AU32" s="3"/>
+      <c r="AV32" s="3"/>
+      <c r="AW32" s="3"/>
+      <c r="AX32" s="3"/>
+      <c r="AY32" s="3"/>
+      <c r="AZ32" s="3"/>
+      <c r="BA32" s="3"/>
+      <c r="BB32" s="3"/>
+      <c r="BC32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="Z1:AD2"/>
-    <mergeCell ref="AH1:AL2"/>
-    <mergeCell ref="AG3:AG10"/>
+    <mergeCell ref="BA19:BB19"/>
+    <mergeCell ref="BA20:BB20"/>
+    <mergeCell ref="BA21:BB21"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="BA8:BB8"/>
+    <mergeCell ref="BA9:BB9"/>
+    <mergeCell ref="BA10:BB10"/>
+    <mergeCell ref="BA15:BB15"/>
+    <mergeCell ref="BA16:BB16"/>
+    <mergeCell ref="BA17:BB17"/>
+    <mergeCell ref="AP12:AT13"/>
+    <mergeCell ref="AH12:AL13"/>
+    <mergeCell ref="AO3:AO10"/>
+    <mergeCell ref="AO14:AO21"/>
+    <mergeCell ref="AS15:AT15"/>
+    <mergeCell ref="AS16:AT16"/>
+    <mergeCell ref="AS17:AT17"/>
+    <mergeCell ref="AS19:AT19"/>
+    <mergeCell ref="AS20:AT20"/>
+    <mergeCell ref="AS21:AT21"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AS6:AT6"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="AS9:AT9"/>
+    <mergeCell ref="AS10:AT10"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AK8:AL8"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AK17:AL17"/>
+    <mergeCell ref="AK19:AL19"/>
+    <mergeCell ref="AK20:AL20"/>
+    <mergeCell ref="AK21:AL21"/>
+    <mergeCell ref="AG14:AG21"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="J12:N13"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="R12:V13"/>
+    <mergeCell ref="AW3:AW10"/>
+    <mergeCell ref="AW14:AW21"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="AK14:AL14"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AS14:AT14"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AP1:AT2"/>
     <mergeCell ref="AX1:BB2"/>
     <mergeCell ref="B12:F13"/>
@@ -3097,118 +3327,27 @@
     <mergeCell ref="BA3:BB3"/>
     <mergeCell ref="BA14:BB14"/>
     <mergeCell ref="AX12:BB13"/>
-    <mergeCell ref="AW3:AW10"/>
-    <mergeCell ref="AW14:AW21"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="AK14:AL14"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AS14:AT14"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="Z1:AD2"/>
+    <mergeCell ref="AH1:AL2"/>
+    <mergeCell ref="AG3:AG10"/>
     <mergeCell ref="AC5:AD5"/>
     <mergeCell ref="AC6:AD6"/>
     <mergeCell ref="AC8:AD8"/>
     <mergeCell ref="AC9:AD9"/>
     <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="R12:V13"/>
-    <mergeCell ref="J12:N13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AK17:AL17"/>
-    <mergeCell ref="AK19:AL19"/>
-    <mergeCell ref="AK20:AL20"/>
-    <mergeCell ref="AK21:AL21"/>
-    <mergeCell ref="AG14:AG21"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AS6:AT6"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="AS9:AT9"/>
-    <mergeCell ref="AS10:AT10"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AK8:AL8"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AP12:AT13"/>
-    <mergeCell ref="AH12:AL13"/>
-    <mergeCell ref="AO3:AO10"/>
-    <mergeCell ref="AO14:AO21"/>
-    <mergeCell ref="AS15:AT15"/>
-    <mergeCell ref="AS16:AT16"/>
-    <mergeCell ref="AS17:AT17"/>
-    <mergeCell ref="AS19:AT19"/>
-    <mergeCell ref="AS20:AT20"/>
-    <mergeCell ref="AS21:AT21"/>
-    <mergeCell ref="BA19:BB19"/>
-    <mergeCell ref="BA20:BB20"/>
-    <mergeCell ref="BA21:BB21"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="BA8:BB8"/>
-    <mergeCell ref="BA9:BB9"/>
-    <mergeCell ref="BA10:BB10"/>
-    <mergeCell ref="BA15:BB15"/>
-    <mergeCell ref="BA16:BB16"/>
-    <mergeCell ref="BA17:BB17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002061008B6BC8FB449E253C883C4CFC30" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e1716c8fb4a3aa10e8089cb6ca6240f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a2e17894-b1f4-4875-ab3b-f8ba29eacc6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1130d71f7c209f5aef10502812f7105" ns3:_="">
     <xsd:import namespace="a2e17894-b1f4-4875-ab3b-f8ba29eacc6c"/>
@@ -3372,31 +3511,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FEF41F8-B27F-423A-B8E6-3E7C85641763}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a2e17894-b1f4-4875-ab3b-f8ba29eacc6c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A6DC354-87C0-41A8-A15C-496869CEE99C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD1A5388-6F2E-4431-BC9E-6FD546B85259}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3412,4 +3542,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A6DC354-87C0-41A8-A15C-496869CEE99C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FEF41F8-B27F-423A-B8E6-3E7C85641763}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a2e17894-b1f4-4875-ab3b-f8ba29eacc6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>